<commit_message>
MUX and EX stage complete
</commit_message>
<xml_diff>
--- a/ALU/FCode.xlsx
+++ b/ALU/FCode.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>add</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>1111</t>
+  </si>
+  <si>
+    <t>math</t>
+  </si>
+  <si>
+    <t>logic</t>
+  </si>
+  <si>
+    <t>0001</t>
   </si>
 </sst>
 </file>
@@ -132,12 +141,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -152,9 +179,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,132 +479,180 @@
     <col min="2" max="2" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C9" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C11" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C12" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C13" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C14" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C15" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>30</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>